<commit_message>
Updated the paths to use the root so it can run even in github
</commit_message>
<xml_diff>
--- a/SeleniumJava/Config/Login.xlsx
+++ b/SeleniumJava/Config/Login.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\Selenium\Java\SeleniumJava\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jun11\git\SeleniumJava\SeleniumJava\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CF3B84-47CF-4AA9-81DA-857DC41BE4C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B2AC95-61AC-41F0-8693-328AC98FAF6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="44">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -500,7 +500,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -542,7 +542,7 @@
       <c r="D2" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -559,7 +559,7 @@
       <c r="D3" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>27</v>
       </c>
     </row>
@@ -576,7 +576,7 @@
       <c r="D4" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>